<commit_message>
switch back to matplotlib
</commit_message>
<xml_diff>
--- a/studying.xlsx
+++ b/studying.xlsx
@@ -23,6 +23,15 @@
     <t>Hours Studied</t>
   </si>
   <si>
+    <t>2024-04-16</t>
+  </si>
+  <si>
+    <t>2024-04-15</t>
+  </si>
+  <si>
+    <t>2024-04-14</t>
+  </si>
+  <si>
     <t>2024-04-13</t>
   </si>
   <si>
@@ -102,15 +111,6 @@
   </si>
   <si>
     <t>2024-03-18</t>
-  </si>
-  <si>
-    <t>2024-03-17</t>
-  </si>
-  <si>
-    <t>2024-03-16</t>
-  </si>
-  <si>
-    <t>2024-03-15</t>
   </si>
   <si>
     <t>Category</t>
@@ -216,94 +216,94 @@
               <c:strCache>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
+                  <c:v>2024-04-16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2024-04-15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2024-04-14</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>2024-04-13</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>2024-04-12</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>2024-04-11</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>2024-04-10</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>2024-04-09</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>2024-04-08</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>2024-04-07</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>2024-04-06</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>2024-04-05</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>2024-04-04</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>2024-04-03</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>2024-04-02</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>2024-04-01</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
                   <c:v>2024-03-31</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="17">
                   <c:v>2024-03-30</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>2024-03-29</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>2024-03-28</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>2024-03-27</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="21">
                   <c:v>2024-03-26</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="22">
                   <c:v>2024-03-25</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="23">
                   <c:v>2024-03-24</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="24">
                   <c:v>2024-03-23</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="25">
                   <c:v>2024-03-22</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="26">
                   <c:v>2024-03-21</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="27">
                   <c:v>2024-03-20</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="28">
                   <c:v>2024-03-19</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="29">
                   <c:v>2024-03-18</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2024-03-17</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2024-03-16</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2024-03-15</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -315,50 +315,50 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>6.666666666666667</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>3.9</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>2.916666666666667</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>1.5</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>0.75</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
                 </c:pt>
@@ -369,16 +369,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>0.75</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0</c:v>
@@ -521,7 +521,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.333333333333333</c:v>
+                  <c:v>0.6666666666666666</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -551,7 +551,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5.333333333333334</c:v>
+                  <c:v>3.333333333333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1012,7 +1012,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>6.666666666666667</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1020,7 +1020,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1028,7 +1028,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>3.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1036,7 +1036,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1044,7 +1044,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1052,7 +1052,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1068,7 +1068,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>2.916666666666667</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1076,7 +1076,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1092,7 +1092,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>1.5</v>
+        <v>2.916666666666667</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1100,7 +1100,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1116,7 +1116,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1124,7 +1124,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1156,7 +1156,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>0.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1180,7 +1180,7 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1274,7 +1274,7 @@
         <v>34</v>
       </c>
       <c r="B2">
-        <v>1.333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1282,7 +1282,7 @@
         <v>35</v>
       </c>
       <c r="B3">
-        <v>5.333333333333334</v>
+        <v>3.333333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update - added other calenders and merged their data together
</commit_message>
<xml_diff>
--- a/studying.xlsx
+++ b/studying.xlsx
@@ -23,6 +23,42 @@
     <t>Hours Studied</t>
   </si>
   <si>
+    <t>2024-07-31</t>
+  </si>
+  <si>
+    <t>2024-07-30</t>
+  </si>
+  <si>
+    <t>2024-07-29</t>
+  </si>
+  <si>
+    <t>2024-07-28</t>
+  </si>
+  <si>
+    <t>2024-07-27</t>
+  </si>
+  <si>
+    <t>2024-07-26</t>
+  </si>
+  <si>
+    <t>2024-07-25</t>
+  </si>
+  <si>
+    <t>2024-07-24</t>
+  </si>
+  <si>
+    <t>2024-07-23</t>
+  </si>
+  <si>
+    <t>2024-07-22</t>
+  </si>
+  <si>
+    <t>2024-07-21</t>
+  </si>
+  <si>
+    <t>2024-07-20</t>
+  </si>
+  <si>
     <t>2024-07-19</t>
   </si>
   <si>
@@ -75,42 +111,6 @@
   </si>
   <si>
     <t>2024-07-02</t>
-  </si>
-  <si>
-    <t>2024-07-01</t>
-  </si>
-  <si>
-    <t>2024-06-30</t>
-  </si>
-  <si>
-    <t>2024-06-29</t>
-  </si>
-  <si>
-    <t>2024-06-28</t>
-  </si>
-  <si>
-    <t>2024-06-27</t>
-  </si>
-  <si>
-    <t>2024-06-26</t>
-  </si>
-  <si>
-    <t>2024-06-25</t>
-  </si>
-  <si>
-    <t>2024-06-24</t>
-  </si>
-  <si>
-    <t>2024-06-23</t>
-  </si>
-  <si>
-    <t>2024-06-22</t>
-  </si>
-  <si>
-    <t>2024-06-21</t>
-  </si>
-  <si>
-    <t>2024-06-20</t>
   </si>
   <si>
     <t>Category</t>
@@ -216,94 +216,94 @@
               <c:strCache>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
+                  <c:v>2024-07-31</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2024-07-30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2024-07-29</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2024-07-28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2024-07-27</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2024-07-26</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2024-07-25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2024-07-24</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2024-07-23</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2024-07-22</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2024-07-21</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2024-07-20</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>2024-07-19</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="13">
                   <c:v>2024-07-18</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="14">
                   <c:v>2024-07-17</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="15">
                   <c:v>2024-07-16</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="16">
                   <c:v>2024-07-15</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="17">
                   <c:v>2024-07-14</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="18">
                   <c:v>2024-07-13</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="19">
                   <c:v>2024-07-12</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="20">
                   <c:v>2024-07-11</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="21">
                   <c:v>2024-07-10</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="22">
                   <c:v>2024-07-09</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="23">
                   <c:v>2024-07-08</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="24">
                   <c:v>2024-07-07</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="25">
                   <c:v>2024-07-06</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="26">
                   <c:v>2024-07-05</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="27">
                   <c:v>2024-07-04</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="28">
                   <c:v>2024-07-03</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="29">
                   <c:v>2024-07-02</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2024-07-01</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2024-06-30</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2024-06-29</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2024-06-28</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2024-06-27</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2024-06-26</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2024-06-25</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2024-06-24</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2024-06-23</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2024-06-22</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2024-06-21</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2024-06-20</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -315,94 +315,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.083333333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>1.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>1.5</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>1.5</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>3.25</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2.25</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.75</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2.583333333333333</c:v>
-                </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.75</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -521,7 +521,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -551,7 +551,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1012,7 +1012,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1020,7 +1020,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1028,7 +1028,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>2.083333333333333</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1036,7 +1036,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1044,7 +1044,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1052,7 +1052,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>1.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1060,7 +1060,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1068,7 +1068,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1084,7 +1084,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1092,7 +1092,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>1.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1108,7 +1108,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>1.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1140,7 +1140,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1148,7 +1148,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1164,7 +1164,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1188,7 +1188,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1204,7 +1204,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>3.25</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1212,7 +1212,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>1.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1220,7 +1220,7 @@
         <v>28</v>
       </c>
       <c r="B28">
-        <v>2.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1228,7 +1228,7 @@
         <v>29</v>
       </c>
       <c r="B29">
-        <v>0.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1236,7 +1236,7 @@
         <v>30</v>
       </c>
       <c r="B30">
-        <v>2.583333333333333</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1244,7 +1244,7 @@
         <v>31</v>
       </c>
       <c r="B31">
-        <v>0.75</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1274,7 +1274,7 @@
         <v>34</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1282,7 +1282,7 @@
         <v>35</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed study time calculation
</commit_message>
<xml_diff>
--- a/studying.xlsx
+++ b/studying.xlsx
@@ -23,6 +23,45 @@
     <t>Hours Studied</t>
   </si>
   <si>
+    <t>2024-08-14</t>
+  </si>
+  <si>
+    <t>2024-08-13</t>
+  </si>
+  <si>
+    <t>2024-08-12</t>
+  </si>
+  <si>
+    <t>2024-08-11</t>
+  </si>
+  <si>
+    <t>2024-08-10</t>
+  </si>
+  <si>
+    <t>2024-08-09</t>
+  </si>
+  <si>
+    <t>2024-08-08</t>
+  </si>
+  <si>
+    <t>2024-08-07</t>
+  </si>
+  <si>
+    <t>2024-08-06</t>
+  </si>
+  <si>
+    <t>2024-08-05</t>
+  </si>
+  <si>
+    <t>2024-08-04</t>
+  </si>
+  <si>
+    <t>2024-08-03</t>
+  </si>
+  <si>
+    <t>2024-08-02</t>
+  </si>
+  <si>
     <t>2024-08-01</t>
   </si>
   <si>
@@ -72,45 +111,6 @@
   </si>
   <si>
     <t>2024-07-16</t>
-  </si>
-  <si>
-    <t>2024-07-15</t>
-  </si>
-  <si>
-    <t>2024-07-14</t>
-  </si>
-  <si>
-    <t>2024-07-13</t>
-  </si>
-  <si>
-    <t>2024-07-12</t>
-  </si>
-  <si>
-    <t>2024-07-11</t>
-  </si>
-  <si>
-    <t>2024-07-10</t>
-  </si>
-  <si>
-    <t>2024-07-09</t>
-  </si>
-  <si>
-    <t>2024-07-08</t>
-  </si>
-  <si>
-    <t>2024-07-07</t>
-  </si>
-  <si>
-    <t>2024-07-06</t>
-  </si>
-  <si>
-    <t>2024-07-05</t>
-  </si>
-  <si>
-    <t>2024-07-04</t>
-  </si>
-  <si>
-    <t>2024-07-03</t>
   </si>
   <si>
     <t>Category</t>
@@ -216,94 +216,94 @@
               <c:strCache>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
+                  <c:v>2024-08-14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2024-08-13</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2024-08-12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2024-08-11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2024-08-10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2024-08-09</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2024-08-08</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2024-08-07</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2024-08-06</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2024-08-05</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2024-08-04</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2024-08-03</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2024-08-02</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>2024-08-01</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="14">
                   <c:v>2024-07-31</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="15">
                   <c:v>2024-07-30</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="16">
                   <c:v>2024-07-29</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="17">
                   <c:v>2024-07-28</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="18">
                   <c:v>2024-07-27</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="19">
                   <c:v>2024-07-26</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="20">
                   <c:v>2024-07-25</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="21">
                   <c:v>2024-07-24</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="22">
                   <c:v>2024-07-23</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="23">
                   <c:v>2024-07-22</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="24">
                   <c:v>2024-07-21</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="25">
                   <c:v>2024-07-20</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="26">
                   <c:v>2024-07-19</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="27">
                   <c:v>2024-07-18</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="28">
                   <c:v>2024-07-17</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="29">
                   <c:v>2024-07-16</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2024-07-15</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2024-07-14</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2024-07-13</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2024-07-12</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2024-07-11</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2024-07-10</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2024-07-09</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2024-07-08</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2024-07-07</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2024-07-06</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2024-07-05</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2024-07-04</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2024-07-03</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -315,70 +315,70 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.833333333333333</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>2.25</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="15">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="16">
                   <c:v>2.083333333333333</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="17">
                   <c:v>0.75</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="18">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>1.75</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="21">
                   <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0</c:v>
@@ -387,10 +387,10 @@
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>0</c:v>
@@ -402,7 +402,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -551,7 +551,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1012,7 +1012,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1020,7 +1020,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>2.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1028,7 +1028,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1036,7 +1036,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>2.083333333333333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1044,7 +1044,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1052,7 +1052,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1068,7 +1068,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>1.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1076,7 +1076,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1084,7 +1084,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>2.833333333333333</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1092,7 +1092,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>1.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1100,7 +1100,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1108,7 +1108,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1116,7 +1116,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1124,7 +1124,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1132,7 +1132,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1140,7 +1140,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>2.083333333333333</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1148,7 +1148,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1156,7 +1156,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>1.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1172,7 +1172,7 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1180,7 +1180,7 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1204,7 +1204,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1212,7 +1212,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>1.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1244,7 +1244,7 @@
         <v>31</v>
       </c>
       <c r="B31">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1282,7 +1282,7 @@
         <v>35</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added studying hours bar graph and subject specific bar graph
</commit_message>
<xml_diff>
--- a/studying.xlsx
+++ b/studying.xlsx
@@ -23,6 +23,9 @@
     <t>Hours Studied</t>
   </si>
   <si>
+    <t>2024-08-16</t>
+  </si>
+  <si>
     <t>2024-08-15</t>
   </si>
   <si>
@@ -108,9 +111,6 @@
   </si>
   <si>
     <t>2024-07-18</t>
-  </si>
-  <si>
-    <t>2024-07-17</t>
   </si>
   <si>
     <t>Category</t>
@@ -216,94 +216,94 @@
               <c:strCache>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
+                  <c:v>2024-08-16</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2024-08-15</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2024-08-14</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>2024-08-13</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>2024-08-12</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>2024-08-11</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>2024-08-10</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>2024-08-09</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>2024-08-08</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>2024-08-07</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>2024-08-06</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>2024-08-05</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>2024-08-04</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>2024-08-03</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>2024-08-02</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>2024-08-01</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>2024-07-31</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>2024-07-30</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>2024-07-29</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>2024-07-28</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>2024-07-27</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>2024-07-26</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>2024-07-25</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>2024-07-24</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>2024-07-23</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>2024-07-22</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>2024-07-21</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>2024-07-20</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>2024-07-19</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>2024-07-18</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2024-07-17</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -315,10 +315,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>5.583333333333334</c:v>
+                  <c:v>4.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>3.083333333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -345,55 +345,55 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>2.833333333333333</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>2.25</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>2.083333333333333</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>0.75</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>1.75</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="23">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>1.5</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>0</c:v>
@@ -521,7 +521,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.333333333333333</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -551,7 +551,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3.25</c:v>
+                  <c:v>4.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1012,7 +1012,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>5.583333333333334</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1020,7 +1020,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>3.083333333333333</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1092,7 +1092,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>2.833333333333333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1100,7 +1100,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>2.833333333333333</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1116,7 +1116,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1124,7 +1124,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1132,7 +1132,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>2.25</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1140,7 +1140,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1148,7 +1148,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>2.083333333333333</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1156,7 +1156,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>0.75</v>
+        <v>2.083333333333333</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1164,7 +1164,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>3</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1172,7 +1172,7 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1180,7 +1180,7 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>1.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1188,7 +1188,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>4</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1196,7 +1196,7 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1204,7 +1204,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>1.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1212,7 +1212,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>3</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1220,7 +1220,7 @@
         <v>28</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1274,7 +1274,7 @@
         <v>34</v>
       </c>
       <c r="B2">
-        <v>2.333333333333333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1282,7 +1282,7 @@
         <v>35</v>
       </c>
       <c r="B3">
-        <v>3.25</v>
+        <v>4.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>